<commit_message>
added missing read_index values
</commit_message>
<xml_diff>
--- a/examples/spreadsheets/v5/filled/SmartSeq2/Q4DemoSS2Metadata_v5.xlsx
+++ b/examples/spreadsheets/v5/filled/SmartSeq2/Q4DemoSS2Metadata_v5.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="29005"/>
-  <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dwelter/Development/HCA/metadata-schema/examples/spreadsheets/v5/filled/SmartSeq2/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="25007"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17620" firstSheet="3" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17620" firstSheet="3" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="project" sheetId="1" r:id="rId1"/>
@@ -24,18 +19,18 @@
   </sheets>
   <calcPr calcId="0" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
-    </ext>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="227">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="227">
   <si>
     <t>A unique label for the project.</t>
   </si>
@@ -1164,7 +1159,7 @@
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="17" customWidth="1"/>
     <col min="2" max="2" width="13" customWidth="1"/>
@@ -1175,7 +1170,7 @@
     <col min="8" max="8" width="21" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1201,7 +1196,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8">
       <c r="A2" s="1" t="s">
         <v>8</v>
       </c>
@@ -1219,7 +1214,7 @@
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8">
       <c r="A3" s="2" t="s">
         <v>12</v>
       </c>
@@ -1245,7 +1240,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8">
       <c r="A4" t="s">
         <v>197</v>
       </c>
@@ -1258,6 +1253,11 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -1269,7 +1269,7 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="12" customWidth="1"/>
     <col min="2" max="2" width="5" customWidth="1"/>
@@ -1280,7 +1280,7 @@
     <col min="8" max="8" width="17" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8">
       <c r="A1" t="s">
         <v>20</v>
       </c>
@@ -1306,7 +1306,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8">
       <c r="A2" s="1" t="s">
         <v>28</v>
       </c>
@@ -1318,7 +1318,7 @@
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8">
       <c r="A3" s="2" t="s">
         <v>29</v>
       </c>
@@ -1344,7 +1344,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8">
       <c r="A4" t="s">
         <v>199</v>
       </c>
@@ -1354,6 +1354,11 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -1365,7 +1370,7 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="14" customWidth="1"/>
     <col min="2" max="2" width="16" customWidth="1"/>
@@ -1393,7 +1398,7 @@
     <col min="25" max="26" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:26">
       <c r="A1" t="s">
         <v>36</v>
       </c>
@@ -1473,7 +1478,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:26">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -1505,7 +1510,7 @@
       <c r="Y2" s="1"/>
       <c r="Z2" s="1"/>
     </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:26">
       <c r="A3" s="2" t="s">
         <v>64</v>
       </c>
@@ -1585,7 +1590,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="4" spans="1:26" s="3" customFormat="1" ht="14" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:26" s="3" customFormat="1" ht="13">
       <c r="A4" s="3" t="s">
         <v>201</v>
       </c>
@@ -1602,12 +1607,17 @@
         <v>152</v>
       </c>
     </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:26">
       <c r="E5" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -1615,11 +1625,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+    <sheetView topLeftCell="F1" workbookViewId="0">
       <selection activeCell="T17" sqref="T17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="14" customWidth="1"/>
     <col min="2" max="2" width="16" customWidth="1"/>
@@ -1639,7 +1649,7 @@
     <col min="16" max="16" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:16">
       <c r="A1" t="s">
         <v>36</v>
       </c>
@@ -1689,7 +1699,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:16">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -1713,7 +1723,7 @@
       <c r="O2" s="1"/>
       <c r="P2" s="1"/>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:16">
       <c r="A3" s="2" t="s">
         <v>64</v>
       </c>
@@ -1763,7 +1773,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="4" spans="1:16" s="3" customFormat="1" ht="14" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:16" s="3" customFormat="1" ht="13">
       <c r="A4" s="3" t="s">
         <v>204</v>
       </c>
@@ -1792,13 +1802,18 @@
         <v>206</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:16">
       <c r="C8" s="3"/>
       <c r="D8" s="3"/>
       <c r="E8" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -1810,7 +1825,7 @@
       <selection activeCell="A31" sqref="A31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="10" customWidth="1"/>
     <col min="2" max="2" width="12" customWidth="1"/>
@@ -1823,7 +1838,7 @@
     <col min="11" max="12" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12">
       <c r="A1" t="s">
         <v>98</v>
       </c>
@@ -1861,7 +1876,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -1885,7 +1900,7 @@
       <c r="K2" s="1"/>
       <c r="L2" s="1"/>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:12">
       <c r="A3" s="2" t="s">
         <v>109</v>
       </c>
@@ -1923,7 +1938,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:12">
       <c r="A4" t="s">
         <v>214</v>
       </c>
@@ -1936,6 +1951,11 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -1947,7 +1967,7 @@
       <selection activeCell="Q4" sqref="Q4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="10" customWidth="1"/>
     <col min="2" max="2" width="12" customWidth="1"/>
@@ -1963,7 +1983,7 @@
     <col min="13" max="14" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14">
       <c r="A1" t="s">
         <v>98</v>
       </c>
@@ -2007,7 +2027,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:14">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -2035,7 +2055,7 @@
       <c r="M2" s="1"/>
       <c r="N2" s="1"/>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:14">
       <c r="A3" s="2" t="s">
         <v>109</v>
       </c>
@@ -2079,7 +2099,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="4" spans="1:14" ht="30" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:14" ht="28">
       <c r="A4" t="s">
         <v>215</v>
       </c>
@@ -2105,6 +2125,11 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -2116,7 +2141,7 @@
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="10" customWidth="1"/>
     <col min="2" max="2" width="12" customWidth="1"/>
@@ -2135,7 +2160,7 @@
     <col min="15" max="17" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:17">
       <c r="A1" t="s">
         <v>98</v>
       </c>
@@ -2188,7 +2213,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:17">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -2217,7 +2242,7 @@
       <c r="P2" s="1"/>
       <c r="Q2" s="1"/>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:17">
       <c r="A3" s="2" t="s">
         <v>109</v>
       </c>
@@ -2270,7 +2295,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:17">
       <c r="A4" t="s">
         <v>222</v>
       </c>
@@ -2289,6 +2314,11 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -2300,7 +2330,7 @@
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="11" customWidth="1"/>
     <col min="2" max="2" width="13" customWidth="1"/>
@@ -2311,7 +2341,7 @@
     <col min="7" max="7" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7">
       <c r="A1" t="s">
         <v>162</v>
       </c>
@@ -2334,7 +2364,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -2347,7 +2377,7 @@
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7">
       <c r="A3" s="2" t="s">
         <v>171</v>
       </c>
@@ -2370,7 +2400,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7">
       <c r="A4" s="4" t="s">
         <v>207</v>
       </c>
@@ -2381,7 +2411,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7">
       <c r="A5" t="s">
         <v>217</v>
       </c>
@@ -2391,6 +2421,11 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -2398,11 +2433,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D37" sqref="D37"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="9" customWidth="1"/>
     <col min="2" max="2" width="11" customWidth="1"/>
@@ -2414,7 +2449,7 @@
     <col min="9" max="9" width="21" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9">
       <c r="A1" t="s">
         <v>178</v>
       </c>
@@ -2443,7 +2478,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -2460,7 +2495,7 @@
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9">
       <c r="A3" s="2" t="s">
         <v>188</v>
       </c>
@@ -2489,13 +2524,16 @@
         <v>195</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9">
       <c r="A4" s="5" t="s">
         <v>211</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>212</v>
       </c>
+      <c r="D4" t="s">
+        <v>187</v>
+      </c>
       <c r="E4" s="5">
         <v>1</v>
       </c>
@@ -2509,12 +2547,15 @@
         <v>210</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9">
       <c r="A5" s="5" t="s">
         <v>213</v>
       </c>
       <c r="B5" s="5" t="s">
         <v>212</v>
+      </c>
+      <c r="D5" t="s">
+        <v>225</v>
       </c>
       <c r="E5" s="5">
         <v>1</v>
@@ -2532,5 +2573,10 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added unknown for biological_sex
</commit_message>
<xml_diff>
--- a/examples/spreadsheets/v5/filled/SmartSeq2/Q4DemoSS2Metadata_v5.xlsx
+++ b/examples/spreadsheets/v5/filled/SmartSeq2/Q4DemoSS2Metadata_v5.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="25007"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17620" firstSheet="3" activeTab="8"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17620" firstSheet="2" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="project" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="227">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="313" uniqueCount="228">
   <si>
     <t>A unique label for the project.</t>
   </si>
@@ -711,6 +711,9 @@
   </si>
   <si>
     <t>5 prime end bias</t>
+  </si>
+  <si>
+    <t>unknown</t>
   </si>
 </sst>
 </file>
@@ -1366,8 +1369,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="W15" sqref="W15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -1605,6 +1608,9 @@
       </c>
       <c r="V4" s="3" t="s">
         <v>152</v>
+      </c>
+      <c r="W4" s="3" t="s">
+        <v>227</v>
       </c>
     </row>
     <row r="5" spans="1:26">
@@ -2433,7 +2439,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>

</xml_diff>